<commit_message>
LBW to H2 analysis for real
</commit_message>
<xml_diff>
--- a/examples/H2_Analysis/landbased_costs_ATB.xlsx
+++ b/examples/H2_Analysis/landbased_costs_ATB.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kbrunik/github/forked/HOPP/examples/H2_Analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cclark2/Desktop/HOPP/HOPP/examples/H2_Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C6FA74-FA21-DF41-A664-480BC81695E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9CC0396-91A7-8D4C-BF50-3312B843657A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25620" yWindow="2000" windowWidth="25620" windowHeight="16000" xr2:uid="{AB22C595-07A8-024E-9552-0DA71A6B15FA}"/>
+    <workbookView xWindow="660" yWindow="460" windowWidth="35180" windowHeight="21940" xr2:uid="{AB22C595-07A8-024E-9552-0DA71A6B15FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -449,7 +449,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>